<commit_message>
chore: fix all test rules
</commit_message>
<xml_diff>
--- a/data/processed/RiskLabel_Yes.xlsx
+++ b/data/processed/RiskLabel_Yes.xlsx
@@ -1045,7 +1045,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
@@ -1315,7 +1315,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -2239,7 +2239,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -3995,7 +3995,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -4349,7 +4349,7 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -4429,7 +4429,7 @@
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -4665,7 +4665,7 @@
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -4707,7 +4707,7 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -4787,7 +4787,7 @@
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Low</t>
         </is>
       </c>
     </row>

</xml_diff>